<commit_message>
AO: SCH/STH mapping may 2021 - improve form 2 and form 3
</commit_message>
<xml_diff>
--- a/SCH-STH/Baseline Mapping/Angola/May 2021/ao_sch_sth_baseline_2_child_kap_202105.xlsx
+++ b/SCH-STH/Baseline Mapping/Angola/May 2021/ao_sch_sth_baseline_2_child_kap_202105.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF05C7DF-EB01-4BB1-AC08-AB8287151F1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CAFE57-55E7-4828-A99A-D726C5AB121A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="838">
   <si>
     <t>type</t>
   </si>
@@ -2533,6 +2533,9 @@
   </si>
   <si>
     <t>selected(${p_didnot_med}, ‘3.Fear of side effects (mention some)’)</t>
+  </si>
+  <si>
+    <t>selected(${p_treatment_worms}, ‘Outros’)</t>
   </si>
 </sst>
 </file>
@@ -2940,10 +2943,10 @@
   <dimension ref="A1:P148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K34" sqref="K34"/>
+      <selection pane="bottomRight" activeCell="K73" sqref="K73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3894,6 +3897,9 @@
       </c>
       <c r="E72" t="s">
         <v>359</v>
+      </c>
+      <c r="K72" t="s">
+        <v>837</v>
       </c>
       <c r="M72" t="s">
         <v>17</v>

</xml_diff>